<commit_message>
new page file created for Add New company and new test added for adding new company
</commit_message>
<xml_diff>
--- a/com.freecrm.uiAutomation/TestData.xlsx
+++ b/com.freecrm.uiAutomation/TestData.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="NewContact" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="NewCompany" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>UserName</t>
   </si>
@@ -55,6 +55,24 @@
   </si>
   <si>
     <t>Sen</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>CompanyStatus</t>
+  </si>
+  <si>
+    <t>LookUpCompanyInput</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Hot</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -436,7 +454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -486,12 +504,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>